<commit_message>
vault, adding Observation Platform table CRUD functionality
</commit_message>
<xml_diff>
--- a/vault/misc/observation-platform.xlsx
+++ b/vault/misc/observation-platform.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="types" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>authority</t>
   </si>
@@ -65,9 +66,6 @@
     <t>CGCFJ</t>
   </si>
   <si>
-    <t>hydrophone</t>
-  </si>
-  <si>
     <t>Transport Canada</t>
   </si>
   <si>
@@ -132,6 +130,39 @@
   </si>
   <si>
     <t>Mistral</t>
+  </si>
+  <si>
+    <t>avion</t>
+  </si>
+  <si>
+    <t>bateau</t>
+  </si>
+  <si>
+    <t>mooring</t>
+  </si>
+  <si>
+    <t>mouillage</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>terre</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>espace</t>
+  </si>
+  <si>
+    <t>underwater glider</t>
+  </si>
+  <si>
+    <t>planeur sous-marin</t>
+  </si>
+  <si>
+    <t>longname</t>
   </si>
 </sst>
 </file>
@@ -449,10 +480,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +585,7 @@
     <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -478,86 +601,89 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -566,56 +692,56 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -624,63 +750,63 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -688,67 +814,67 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
         <v>29</v>
-      </c>
-      <c r="E18" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to Excel file with platforms
</commit_message>
<xml_diff>
--- a/vault/misc/observation-platform.xlsx
+++ b/vault/misc/observation-platform.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>authority</t>
   </si>
@@ -163,19 +163,31 @@
   </si>
   <si>
     <t>longname</t>
+  </si>
+  <si>
+    <t>Transport Canada Dash 7 - CGCFR</t>
+  </si>
+  <si>
+    <t>Transport Canada Dash 8 - CGCFJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,8 +210,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +588,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -657,8 +670,11 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -673,6 +689,9 @@
       </c>
       <c r="E6" t="s">
         <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>